<commit_message>
updated calendar and change to is None
</commit_message>
<xml_diff>
--- a/bssr_calendar/TRI_2_Calendar.xlsx
+++ b/bssr_calendar/TRI_2_Calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flynnlambrechts/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flynnlambrechts/Desktop/Coding/BssrBot2/BssrBot-Dev/bssr_calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A89DA838-A01E-9241-95A5-43C1A56551DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C46D32F-AE0C-AC4B-AE25-B0E1D73E61DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRI_2_Calendar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>Silly Season</t>
   </si>
@@ -173,13 +173,37 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>WholeWeek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,6 +334,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1015,224 +1045,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>50</v>
@@ -1241,58 +1275,58 @@
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>50</v>
@@ -1301,26 +1335,56 @@
         <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J10" s="1"/>
     </row>
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>